<commit_message>
all rules are now working
</commit_message>
<xml_diff>
--- a/Checks/DAF Validator V1.xlsx
+++ b/Checks/DAF Validator V1.xlsx
@@ -8,10 +8,10 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Feuil1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Feuil1!$1:$81</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Feuil1!$1:$149</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -388,7 +388,7 @@
     <t xml:space="preserve">element X should be a least connected with a element Y</t>
   </si>
   <si>
-    <t xml:space="preserve">dActor 	 isPerformedBy 	 dRole</t>
+    <t xml:space="preserve">dActor isPerformedBy dRole</t>
   </si>
   <si>
     <t xml:space="preserve">dActor 	 participatesIn 	 dBusinessUseCase</t>
@@ -752,87 +752,87 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -850,6 +850,22 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFBFBFBF"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -857,21 +873,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -879,6 +881,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF00B050"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -886,6 +889,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -957,33 +961,139 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:J149"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B128" activeCellId="0" sqref="B128"/>
+      <selection pane="bottomLeft" activeCell="B89" activeCellId="0" sqref="B89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="77.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="77.13"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.42"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="11.42"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="11.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="4" width="6.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="7.87"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="9" style="1" width="11.42"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="7.88"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="9" style="1" width="11.43"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="true" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="5" customFormat="true" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1070,7 +1180,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A5" s="12"/>
       <c r="B5" s="13"/>
       <c r="D5" s="1" t="s">
@@ -1092,7 +1202,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A6" s="12"/>
       <c r="B6" s="13"/>
       <c r="D6" s="1" t="s">
@@ -1114,7 +1224,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A7" s="12"/>
       <c r="B7" s="13"/>
       <c r="D7" s="1" t="s">
@@ -1310,7 +1420,7 @@
       <c r="B16" s="16"/>
       <c r="E16" s="14"/>
     </row>
-    <row r="17" customFormat="false" ht="30" hidden="true" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="17" customFormat="false" ht="23.85" hidden="true" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A17" s="4"/>
       <c r="B17" s="2" t="s">
         <v>32</v>
@@ -1337,7 +1447,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A18" s="4"/>
       <c r="E18" s="14"/>
       <c r="F18" s="4" t="n">
@@ -1353,7 +1463,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A19" s="4"/>
       <c r="B19" s="2" t="s">
         <v>34</v>
@@ -1555,7 +1665,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="30" hidden="true" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="27" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A27" s="4"/>
       <c r="B27" s="2" t="s">
         <v>47</v>
@@ -1579,7 +1689,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A28" s="4"/>
       <c r="B28" s="2" t="s">
         <v>49</v>
@@ -1915,7 +2025,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A43" s="20"/>
       <c r="B43" s="13"/>
       <c r="E43" s="14"/>
@@ -2100,7 +2210,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" s="1" customFormat="true" ht="30" hidden="true" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="51" s="1" customFormat="true" ht="23.85" hidden="true" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A51" s="20"/>
       <c r="B51" s="13"/>
       <c r="C51" s="2" t="s">
@@ -2850,7 +2960,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="2" t="s">
         <v>121</v>
       </c>
@@ -2858,7 +2968,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="2" t="s">
         <v>122</v>
       </c>
@@ -2866,7 +2976,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="2" t="s">
         <v>123</v>
       </c>
@@ -2874,7 +2984,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="2" t="s">
         <v>124</v>
       </c>
@@ -2882,7 +2992,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="2" t="s">
         <v>125</v>
       </c>
@@ -2890,7 +3000,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="2" t="s">
         <v>126</v>
       </c>
@@ -2898,7 +3008,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="2" t="s">
         <v>127</v>
       </c>
@@ -2906,7 +3016,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="2" t="s">
         <v>128</v>
       </c>
@@ -2914,7 +3024,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B91" s="2" t="s">
         <v>129</v>
       </c>
@@ -2922,7 +3032,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B92" s="2" t="s">
         <v>130</v>
       </c>
@@ -2930,7 +3040,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B93" s="2" t="s">
         <v>131</v>
       </c>
@@ -2938,7 +3048,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="2" t="s">
         <v>132</v>
       </c>
@@ -2946,7 +3056,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B95" s="2" t="s">
         <v>133</v>
       </c>
@@ -2954,7 +3064,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="2" t="s">
         <v>134</v>
       </c>
@@ -2962,7 +3072,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="2" t="s">
         <v>135</v>
       </c>
@@ -2970,7 +3080,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B98" s="2" t="s">
         <v>136</v>
       </c>
@@ -2978,7 +3088,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="2" t="s">
         <v>137</v>
       </c>
@@ -2986,7 +3096,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="2" t="s">
         <v>138</v>
       </c>
@@ -2994,7 +3104,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B101" s="2" t="s">
         <v>139</v>
       </c>
@@ -3002,7 +3112,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B102" s="2" t="s">
         <v>140</v>
       </c>
@@ -3010,7 +3120,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B103" s="2" t="s">
         <v>141</v>
       </c>
@@ -3018,7 +3128,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B104" s="2" t="s">
         <v>142</v>
       </c>
@@ -3026,7 +3136,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B105" s="2" t="s">
         <v>143</v>
       </c>
@@ -3034,7 +3144,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B106" s="2" t="s">
         <v>144</v>
       </c>
@@ -3042,7 +3152,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B107" s="2" t="s">
         <v>145</v>
       </c>
@@ -3050,7 +3160,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="2" t="s">
         <v>146</v>
       </c>
@@ -3058,7 +3168,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B109" s="2" t="s">
         <v>147</v>
       </c>
@@ -3066,7 +3176,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B110" s="2" t="s">
         <v>148</v>
       </c>
@@ -3074,7 +3184,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B111" s="2" t="s">
         <v>149</v>
       </c>
@@ -3082,7 +3192,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B112" s="2" t="s">
         <v>150</v>
       </c>
@@ -3090,7 +3200,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="2" t="s">
         <v>151</v>
       </c>
@@ -3098,7 +3208,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B114" s="2" t="s">
         <v>152</v>
       </c>
@@ -3106,7 +3216,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B115" s="2" t="s">
         <v>153</v>
       </c>
@@ -3114,7 +3224,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B116" s="2" t="s">
         <v>154</v>
       </c>
@@ -3122,7 +3232,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B117" s="2" t="s">
         <v>155</v>
       </c>
@@ -3130,7 +3240,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B118" s="2" t="s">
         <v>156</v>
       </c>
@@ -3138,7 +3248,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B119" s="2" t="s">
         <v>157</v>
       </c>
@@ -3146,7 +3256,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B120" s="2" t="s">
         <v>158</v>
       </c>
@@ -3154,7 +3264,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B121" s="2" t="s">
         <v>159</v>
       </c>
@@ -3162,7 +3272,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B122" s="2" t="s">
         <v>160</v>
       </c>
@@ -3170,7 +3280,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B123" s="2" t="s">
         <v>161</v>
       </c>
@@ -3178,7 +3288,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B124" s="2" t="s">
         <v>162</v>
       </c>
@@ -3186,7 +3296,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B125" s="2" t="s">
         <v>163</v>
       </c>
@@ -3194,7 +3304,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B126" s="2" t="s">
         <v>164</v>
       </c>
@@ -3202,7 +3312,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B127" s="2" t="s">
         <v>165</v>
       </c>
@@ -3210,7 +3320,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B128" s="2" t="s">
         <v>166</v>
       </c>
@@ -3218,7 +3328,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B129" s="2" t="s">
         <v>167</v>
       </c>
@@ -3226,7 +3336,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B130" s="2" t="s">
         <v>168</v>
       </c>
@@ -3234,7 +3344,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B131" s="2" t="s">
         <v>169</v>
       </c>
@@ -3242,7 +3352,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B132" s="2" t="s">
         <v>170</v>
       </c>
@@ -3250,7 +3360,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B133" s="2" t="s">
         <v>171</v>
       </c>
@@ -3258,7 +3368,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B134" s="2" t="s">
         <v>172</v>
       </c>
@@ -3266,7 +3376,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B135" s="2" t="s">
         <v>173</v>
       </c>
@@ -3274,7 +3384,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B136" s="2" t="s">
         <v>174</v>
       </c>
@@ -3282,7 +3392,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B137" s="2" t="s">
         <v>175</v>
       </c>
@@ -3290,7 +3400,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B138" s="2" t="s">
         <v>176</v>
       </c>
@@ -3298,7 +3408,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B139" s="2" t="s">
         <v>177</v>
       </c>
@@ -3306,7 +3416,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B140" s="2" t="s">
         <v>178</v>
       </c>
@@ -3314,7 +3424,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B141" s="2" t="s">
         <v>179</v>
       </c>
@@ -3322,7 +3432,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B142" s="2" t="s">
         <v>180</v>
       </c>
@@ -3330,7 +3440,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B143" s="2" t="s">
         <v>181</v>
       </c>
@@ -3338,7 +3448,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B144" s="2" t="s">
         <v>182</v>
       </c>
@@ -3346,7 +3456,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B145" s="2" t="s">
         <v>183</v>
       </c>
@@ -3354,7 +3464,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B146" s="2" t="s">
         <v>184</v>
       </c>
@@ -3362,7 +3472,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B147" s="2" t="s">
         <v>185</v>
       </c>
@@ -3370,7 +3480,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B148" s="2" t="s">
         <v>186</v>
       </c>
@@ -3378,7 +3488,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B149" s="2" t="s">
         <v>187</v>
       </c>
@@ -3387,7 +3497,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="1:81">
+  <autoFilter ref="1:149">
     <filterColumn colId="4">
       <filters blank="1">
         <filter val="Yes"/>

</xml_diff>